<commit_message>
Upload a revised excel file
Uploading a revised excel file for testing
</commit_message>
<xml_diff>
--- a/GHE_test.xlsx
+++ b/GHE_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>before revised</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Revised!</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -347,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2"/>
+  <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -360,6 +364,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>